<commit_message>
populate best athlete map dynamically
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/competitionBook/Scores-LETTER.xlsx
+++ b/owlcms/src/main/resources/templates/competitionBook/Scores-LETTER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\competitionBook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698928F9-DC5F-4BC8-BC3F-94EEFD8B7B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539E5A62-65DF-4B16-BAD7-075665E7B429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="4065" windowWidth="23205" windowHeight="11295" tabRatio="447" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="447" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C" sheetId="35" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="149">
   <si>
     <t>${l.lastName}</t>
   </si>
@@ -494,6 +494,9 @@
   </si>
   <si>
     <t>${t.get("Category")}</t>
+  </si>
+  <si>
+    <t>${bestRankingTitle}</t>
   </si>
 </sst>
 </file>
@@ -6134,7 +6137,7 @@
   </sheetPr>
   <dimension ref="A1:Z107"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
@@ -8796,8 +8799,8 @@
   </sheetPr>
   <dimension ref="A1:V102"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8862,7 +8865,7 @@
         <v>48</v>
       </c>
       <c r="R1" s="104" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="S1" s="104"/>
       <c r="U1"/>
@@ -9350,7 +9353,7 @@
   <dimension ref="A1:S97"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="R1" sqref="R1:S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9413,7 +9416,7 @@
         <v>48</v>
       </c>
       <c r="R1" s="104" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="S1" s="104"/>
     </row>

</xml_diff>